<commit_message>
updated excel input for farm fields
</commit_message>
<xml_diff>
--- a/RISF/Input_Template_Farm_new.xlsx
+++ b/RISF/Input_Template_Farm_new.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgOXkMZtGU4wppLr6ks18rMy7xhLw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgl/ZCBBDhzVLJ7q9DYS8koQtvoIw=="/>
     </ext>
   </extLst>
 </workbook>
@@ -326,7 +326,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -337,10 +337,10 @@
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="top"/>
+      <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="11" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
@@ -606,9 +606,7 @@
     <col customWidth="1" min="1" max="1" width="18.75"/>
     <col customWidth="1" min="2" max="2" width="21.63"/>
     <col customWidth="1" min="3" max="3" width="62.75"/>
-    <col customWidth="1" min="4" max="4" width="12.63"/>
     <col customWidth="1" min="5" max="5" width="19.38"/>
-    <col customWidth="1" min="6" max="6" width="12.63"/>
     <col customWidth="1" min="7" max="7" width="48.63"/>
   </cols>
   <sheetData>
@@ -671,7 +669,7 @@
       <c r="A5" s="7">
         <v>3.0</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -787,13 +785,13 @@
       <c r="C12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="12" t="s">
         <v>30</v>
       </c>
     </row>
@@ -801,8 +799,8 @@
       <c r="A13" s="7">
         <v>11.0</v>
       </c>
-      <c r="B13" s="8">
-        <v>2.5</v>
+      <c r="B13" s="13">
+        <v>1.5</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>31</v>
@@ -816,7 +814,7 @@
       <c r="G13" s="15">
         <v>1.099974368E7</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -832,7 +830,7 @@
       <c r="G14" s="15">
         <v>-94670.03997</v>
       </c>
-      <c r="H14" s="13"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="B15" s="2"/>
@@ -846,7 +844,7 @@
       <c r="G15" s="15">
         <v>130.7782628</v>
       </c>
-      <c r="H15" s="13"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="B16" s="2"/>
@@ -860,7 +858,7 @@
       <c r="G16" s="15">
         <v>-0.050682689</v>
       </c>
-      <c r="H16" s="13"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="B17" s="2"/>
@@ -874,7 +872,7 @@
       <c r="G17" s="16">
         <v>-2.17522E-7</v>
       </c>
-      <c r="H17" s="13"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="B18" s="2"/>
@@ -890,10 +888,10 @@
     <row r="20" ht="15.75" customHeight="1">
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="12" t="s">
         <v>45</v>
       </c>
     </row>
@@ -952,13 +950,13 @@
     <row r="27" ht="15.75" customHeight="1">
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -974,7 +972,7 @@
       <c r="G28" s="15">
         <v>142.7942484</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="12" t="s">
         <v>30</v>
       </c>
     </row>
@@ -990,7 +988,7 @@
       <c r="G29" s="16">
         <v>-1.65183E-5</v>
       </c>
-      <c r="H29" s="13"/>
+      <c r="H29" s="12"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="B30" s="2"/>
@@ -1004,7 +1002,7 @@
       <c r="G30" s="16">
         <v>4.68247E-13</v>
       </c>
-      <c r="H30" s="13"/>
+      <c r="H30" s="12"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="B31" s="2"/>
@@ -1018,7 +1016,7 @@
       <c r="G31" s="16">
         <v>-1.76119E-20</v>
       </c>
-      <c r="H31" s="13"/>
+      <c r="H31" s="12"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="B32" s="2"/>
@@ -1032,7 +1030,7 @@
       <c r="G32" s="16">
         <v>3.88805E-28</v>
       </c>
-      <c r="H32" s="13"/>
+      <c r="H32" s="12"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="B33" s="2"/>

</xml_diff>